<commit_message>
Extracting t_red from t_tkn
</commit_message>
<xml_diff>
--- a/Classeur2.xlsx
+++ b/Classeur2.xlsx
@@ -538,13 +538,13 @@
     <t>[digits|&amp;]&gt;{&amp;digits|file}</t>
   </si>
   <si>
-    <t>[digits|&amp;]&gt;&gt;{&amp;digits|file}</t>
-  </si>
-  <si>
     <t>[digits]&lt;{&amp;digits|file}</t>
   </si>
   <si>
-    <t>[digits]&lt;&lt;{&amp;digits|file}</t>
+    <t>[digits]&gt;&gt;file</t>
+  </si>
+  <si>
+    <t>[digits]&lt;&lt;keyword</t>
   </si>
 </sst>
 </file>
@@ -631,9 +631,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="163">
+  <cellStyleXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -808,7 +810,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="163">
+  <cellStyles count="165">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="3" builtinId="9" hidden="1"/>
@@ -971,6 +973,8 @@
     <cellStyle name="Lien hypertexte visité" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="161" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1560,8 +1564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E17:R136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="K136" sqref="K136"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="K133" sqref="K133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1980,12 +1984,12 @@
     </row>
     <row r="120" spans="11:11">
       <c r="K120" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="121" spans="11:11">
       <c r="K121" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="122" spans="11:11">

</xml_diff>